<commit_message>
start implementing routine for var eff
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzer.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzer.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/dahe23af_student_cbs_dk/Documents/Dokumente/GitHub/Nord_H2ub/Spine_Projects/Input_data/Input_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD8282B4-9216-48A4-B111-A8343976357E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046BDF9C-14DC-4C73-8529-F59D1FAC7293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency Electrolyzer" sheetId="1" r:id="rId1"/>
+    <sheet name="Idea_Implementation" sheetId="3" r:id="rId2"/>
+    <sheet name="Test_Adjustment" sheetId="4" r:id="rId3"/>
+    <sheet name="Source" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Efficiency Electrolyzer'!$G$4</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Efficiency Electrolyzer'!$H$4</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">"0,0001"</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -30,7 +33,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Efficiency Electrolyzer'!$G$5</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Efficiency Electrolyzer'!$H$5</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">"0,000001"</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -44,15 +47,25 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Power [MW]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Efficiency [kg/MWh]</t>
   </si>
@@ -65,14 +78,59 @@
   <si>
     <t>Angepasster Wirkungsgrad</t>
   </si>
+  <si>
+    <t>Source: https://www.sciencedirect.com/science/article/pii/S0098135423003204</t>
+  </si>
+  <si>
+    <t>Average_Eff</t>
+  </si>
+  <si>
+    <t>Power Kasso [MW]</t>
+  </si>
+  <si>
+    <t>Power [%]</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>Share Capacity</t>
+  </si>
+  <si>
+    <t>Remaining Capacity</t>
+  </si>
+  <si>
+    <t>Share Capcity Rounded</t>
+  </si>
+  <si>
+    <t>Remaining Capacity Rounded</t>
+  </si>
+  <si>
+    <t>Slices</t>
+  </si>
+  <si>
+    <t>Operating Points</t>
+  </si>
+  <si>
+    <t>Efficiency_tobe</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>EFF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -552,13 +610,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -629,17 +686,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E36" totalsRowShown="0">
-  <autoFilter ref="A1:E36"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Power [MW]"/>
-    <tableColumn id="2" name="Efficiency [kg/MWh]"/>
-    <tableColumn id="3" name="Wirkungsgrad" dataDxfId="2" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F36" totalsRowShown="0">
+  <autoFilter ref="A1:F36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="6" xr3:uid="{0A06C26B-7249-4F9D-98BF-709113EE2094}" name="Power [%]">
+      <calculatedColumnFormula>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Power Kasso [MW]"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Efficiency [kg/MWh]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Wirkungsgrad" dataDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Change in Power" dataDxfId="1"/>
-    <tableColumn id="5" name="Angepasster Wirkungsgrad" dataDxfId="0">
-      <calculatedColumnFormula>(Table1[[#This Row],[Wirkungsgrad]]-Table1[[#This Row],[Change in Power]]*C1)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Change in Power" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Angepasster Wirkungsgrad" dataDxfId="0">
+      <calculatedColumnFormula>(Table1[[#This Row],[Wirkungsgrad]]-Table1[[#This Row],[Change in Power]]*D1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -942,746 +1002,891 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
         <v>0</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>18.600000000000001</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.61993799999999999</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
         <v>0.61990000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>5.198960207958409E-3</v>
+      </c>
+      <c r="B3">
         <v>0.26</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>18.739999999999998</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.62460419999999994</v>
       </c>
-      <c r="D3" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A2</f>
+      <c r="E3">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B2</f>
         <v>0.26</v>
       </c>
-      <c r="E3" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D2)-D2*E2)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F3" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E2)-E2*F2)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.62460419999999994</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>1.2797440511897622E-2</v>
+      </c>
+      <c r="B4">
         <v>0.64</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>18.87</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.62893710000000003</v>
       </c>
-      <c r="D4" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A3</f>
+      <c r="E4">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B3</f>
         <v>0.38</v>
       </c>
-      <c r="E4" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D3)-D3*E3)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F4" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E3)-E3*F3)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.63190171578947374</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H4" s="3"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>2.0595880823835233E-2</v>
+      </c>
+      <c r="B5">
         <v>1.03</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>19.010000000000002</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.63360329999999998</v>
       </c>
-      <c r="D5" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A4</f>
+      <c r="E5">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B4</f>
         <v>0.39</v>
       </c>
-      <c r="E5" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D4)-D4*E4)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F5" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E4)-E4*F4)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.63526125384615373</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>2.8194361127774445E-2</v>
+      </c>
+      <c r="B6">
         <v>1.41</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>19.13</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.63760289999999997</v>
       </c>
-      <c r="D6" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A5</f>
+      <c r="E6">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B5</f>
         <v>0.37999999999999989</v>
       </c>
-      <c r="E6" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D5)-D5*E5)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F6" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E5)-E5*F5)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.64000616842105262</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>3.5992801439712063E-2</v>
+      </c>
+      <c r="B7">
         <v>1.8</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>19.260000000000002</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.64193580000000006</v>
       </c>
-      <c r="D7" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A6</f>
+      <c r="E7">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B6</f>
         <v>0.39000000000000012</v>
       </c>
-      <c r="E7" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D6)-D6*E6)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F7" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E6)-E6*F6)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.64381595384615398</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>4.8790241951609678E-2</v>
+      </c>
+      <c r="B8">
         <v>2.44</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>19.39</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.64626870000000003</v>
       </c>
-      <c r="D8" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A7</f>
+      <c r="E8">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B7</f>
         <v>0.6399999999999999</v>
       </c>
-      <c r="E8" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D7)-D7*E7)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F8" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E7)-E7*F7)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.64776334218749998</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>6.4187162567486508E-2</v>
+      </c>
+      <c r="B9">
         <v>3.21</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>19.52</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.6506016</v>
       </c>
-      <c r="D9" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A8</f>
+      <c r="E9">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B8</f>
         <v>0.77</v>
       </c>
-      <c r="E9" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D8)-D8*E8)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F9" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E8)-E8*F8)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.65296067142857139</v>
       </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>8.3383323335332937E-2</v>
+      </c>
+      <c r="B10">
         <v>4.17</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>19.64</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.65460119999999999</v>
       </c>
-      <c r="D10" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A9</f>
+      <c r="E10">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B9</f>
         <v>0.96</v>
       </c>
-      <c r="E10" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D9)-D9*E9)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F10" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E9)-E9*F9)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.65591704062499989</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.10397920415916817</v>
+      </c>
+      <c r="B11">
         <v>5.2</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>19.72</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.65726759999999995</v>
       </c>
-      <c r="D11" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A10</f>
+      <c r="E11">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B10</f>
         <v>1.0300000000000002</v>
       </c>
-      <c r="E11" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D10)-D10*E10)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F11" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E10)-E10*F10)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.65852637378640788</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.13077384523095381</v>
+      </c>
+      <c r="B12">
         <v>6.54</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>19.78</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.65926740000000006</v>
       </c>
-      <c r="D12" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A11</f>
+      <c r="E12">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B11</f>
         <v>1.3399999999999999</v>
       </c>
-      <c r="E12" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D11)-D11*E11)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F12" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E11)-E11*F11)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.65983699477611935</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.15396920615876825</v>
+      </c>
+      <c r="B13">
         <v>7.7</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>19.78</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.65926740000000006</v>
       </c>
-      <c r="D13" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A12</f>
+      <c r="E13">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B12</f>
         <v>1.1600000000000001</v>
       </c>
-      <c r="E13" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D12)-D12*E12)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F13" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E12)-E12*F12)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.65860941982758647</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.18216356728654268</v>
+      </c>
+      <c r="B14">
         <v>9.11</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>19.77</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.65893409999999997</v>
       </c>
-      <c r="D14" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A13</f>
+      <c r="E14">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B13</f>
         <v>1.4099999999999993</v>
       </c>
-      <c r="E14" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D13)-D13*E13)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F14" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E13)-E13*F13)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.65920121276595722</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.21035792841431714</v>
+      </c>
+      <c r="B15">
         <v>10.52</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>19.73</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.65760089999999993</v>
       </c>
-      <c r="D15" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A14</f>
+      <c r="E15">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B14</f>
         <v>1.4100000000000001</v>
       </c>
-      <c r="E15" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D14)-D14*E14)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F15" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E14)-E14*F14)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.65600058723404253</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.24495100979804041</v>
+      </c>
+      <c r="B16">
         <v>12.25</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>19.670000000000002</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.65560110000000005</v>
       </c>
-      <c r="D16" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A15</f>
+      <c r="E16">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B15</f>
         <v>1.7300000000000004</v>
       </c>
-      <c r="E16" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D15)-D15*E15)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F16" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E15)-E15*F15)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.6552755063583815</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.27814437112577484</v>
+      </c>
+      <c r="B17">
         <v>13.91</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>19.579999999999998</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.65260139999999989</v>
       </c>
-      <c r="D17" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A16</f>
+      <c r="E17">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B16</f>
         <v>1.6600000000000001</v>
       </c>
-      <c r="E17" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D16)-D16*E16)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F17" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E16)-E16*F16)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.64981453012048151</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.31413717256548696</v>
+      </c>
+      <c r="B18">
         <v>15.71</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>19.489999999999998</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.64960169999999995</v>
       </c>
-      <c r="D18" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A17</f>
+      <c r="E18">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B17</f>
         <v>1.8000000000000007</v>
       </c>
-      <c r="E18" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D17)-D17*E17)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F18" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E17)-E17*F17)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.64940542333333351</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.34233153369326136</v>
+      </c>
+      <c r="B19">
         <v>17.12</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>19.399999999999999</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.6466019999999999</v>
       </c>
-      <c r="D19" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A18</f>
+      <c r="E19">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B18</f>
         <v>1.4100000000000001</v>
       </c>
-      <c r="E19" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D18)-D18*E18)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F19" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E18)-E18*F18)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.64302316170212737</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.37832433513297348</v>
+      </c>
+      <c r="B20">
         <v>18.920000000000002</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>19.3</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.64326899999999998</v>
       </c>
-      <c r="D20" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A19</f>
+      <c r="E20">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B19</f>
         <v>1.8000000000000007</v>
       </c>
-      <c r="E20" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D19)-D19*E19)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F20" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E19)-E19*F19)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.64346157333333365</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.40891821635672865</v>
+      </c>
+      <c r="B21">
         <v>20.45</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>19.2</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.63993599999999995</v>
       </c>
-      <c r="D21" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A20</f>
+      <c r="E21">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B20</f>
         <v>1.5299999999999976</v>
       </c>
-      <c r="E21" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D20)-D20*E20)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F21" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E20)-E20*F20)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.63578826666666621</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.44111177764447107</v>
+      </c>
+      <c r="B22">
         <v>22.06</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>19.100000000000001</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.63660300000000003</v>
       </c>
-      <c r="D22" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A21</f>
+      <c r="E22">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B21</f>
         <v>1.6099999999999994</v>
       </c>
-      <c r="E22" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D21)-D21*E21)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F22" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E21)-E21*F21)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.63737724968944143</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.47190561887622479</v>
+      </c>
+      <c r="B23">
         <v>23.6</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>19.010000000000002</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.63360329999999998</v>
       </c>
-      <c r="D23" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A22</f>
+      <c r="E23">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B22</f>
         <v>1.5400000000000027</v>
       </c>
-      <c r="E23" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D22)-D22*E22)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F23" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E22)-E22*F22)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.62965780714285668</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.50009998000399924</v>
+      </c>
+      <c r="B24">
         <v>25.01</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>18.920000000000002</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.63060360000000004</v>
       </c>
-      <c r="D24" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A23</f>
+      <c r="E24">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B23</f>
         <v>1.4100000000000001</v>
       </c>
-      <c r="E24" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D23)-D23*E23)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F24" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E23)-E23*F23)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.63163659361702185</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.53069386122775442</v>
+      </c>
+      <c r="B25">
         <v>26.54</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>18.829999999999998</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.62760389999999988</v>
       </c>
-      <c r="D25" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A24</f>
+      <c r="E25">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B24</f>
         <v>1.5299999999999976</v>
       </c>
-      <c r="E25" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D24)-D24*E24)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F25" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E24)-E24*F24)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.62388749607843064</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.5654869026194761</v>
+      </c>
+      <c r="B26">
         <v>28.28</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>18.72</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.62393759999999998</v>
       </c>
-      <c r="D26" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A25</f>
+      <c r="E26">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B25</f>
         <v>1.740000000000002</v>
       </c>
-      <c r="E26" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D25)-D25*E25)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F26" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E25)-E25*F25)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.62398165689655227</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.60647870425914818</v>
+      </c>
+      <c r="B27">
         <v>30.33</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>18.600000000000001</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.61993799999999999</v>
       </c>
-      <c r="D27" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A26</f>
+      <c r="E27">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B26</f>
         <v>2.0499999999999972</v>
       </c>
-      <c r="E27" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D26)-D26*E26)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F27" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E26)-E26*F26)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.61650582292682887</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.64867026594681065</v>
+      </c>
+      <c r="B28">
         <v>32.44</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>18.47</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.61560509999999991</v>
       </c>
-      <c r="D28" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A27</f>
+      <c r="E28">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B27</f>
         <v>2.1099999999999994</v>
       </c>
-      <c r="E28" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D27)-D27*E27)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F28" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E27)-E27*F27)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.61472999004739348</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.68966206758648274</v>
+      </c>
+      <c r="B29">
         <v>34.49</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>18.36</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.6119388</v>
       </c>
-      <c r="D29" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A28</f>
+      <c r="E29">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B28</f>
         <v>2.0500000000000043</v>
       </c>
-      <c r="E29" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D28)-D28*E28)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F29" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E28)-E28*F28)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.60906591658536569</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.73725254949010199</v>
+      </c>
+      <c r="B30">
         <v>36.869999999999997</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>18.22</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.60727259999999994</v>
       </c>
-      <c r="D30" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A29</f>
+      <c r="E30">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B29</f>
         <v>2.3799999999999955</v>
       </c>
-      <c r="E30" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D29)-D29*E29)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F30" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E29)-E29*F29)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.60572793655462187</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.78724255148970201</v>
+      </c>
+      <c r="B31">
         <v>39.369999999999997</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>18.079999999999998</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.60260639999999988</v>
       </c>
-      <c r="D31" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A30</f>
+      <c r="E31">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B30</f>
         <v>2.5</v>
       </c>
-      <c r="E31" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D30)-D30*E30)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F31" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E30)-E30*F30)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.59963469719999973</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.83583283343331327</v>
+      </c>
+      <c r="B32">
         <v>41.8</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>17.96</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.59860679999999999</v>
       </c>
-      <c r="D32" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A31</f>
+      <c r="E32">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B31</f>
         <v>2.4299999999999997</v>
       </c>
-      <c r="E32" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D31)-D31*E31)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F32" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E31)-E31*F31)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.59754929259259293</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.88082383523295338</v>
+      </c>
+      <c r="B33">
         <v>44.05</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>17.84</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.5946072</v>
       </c>
-      <c r="D33" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A32</f>
+      <c r="E33">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B32</f>
         <v>2.25</v>
       </c>
-      <c r="E33" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D32)-D32*E32)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F33" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E32)-E32*F32)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.59142973999999959</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.92561487702459511</v>
+      </c>
+      <c r="B34">
         <v>46.29</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>17.73</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D34" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.59094089999999999</v>
       </c>
-      <c r="D34" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A33</f>
+      <c r="E34">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B33</f>
         <v>2.240000000000002</v>
       </c>
-      <c r="E34" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D33)-D33*E33)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F34" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E33)-E33*F33)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.59044987767857182</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>0.96020795840831841</v>
+      </c>
+      <c r="B35">
         <v>48.02</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>17.63</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.58760789999999996</v>
       </c>
-      <c r="D35" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A34</f>
+      <c r="E35">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B34</f>
         <v>1.730000000000004</v>
       </c>
-      <c r="E35" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D34)-D34*E34)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F35" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E34)-E34*F34)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.58392811387283194</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]/$B$36</f>
+        <v>1</v>
+      </c>
+      <c r="B36">
         <v>50.01</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>17.55</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D36" s="1">
         <f>Table1[[#This Row],[Efficiency '[kg/MWh']]]*0.03333</f>
         <v>0.5849415</v>
       </c>
-      <c r="D36" s="3">
-        <f>Table1[[#This Row],[Power '[MW']]]-A35</f>
+      <c r="E36">
+        <f>Table1[[#This Row],[Power Kasso '[MW']]]-B35</f>
         <v>1.9899999999999949</v>
       </c>
-      <c r="E36" s="2">
-        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+D35)-D35*E35)/Table1[[#This Row],[Change in Power]]</f>
+      <c r="F36" s="2">
+        <f>(Table1[[#This Row],[Wirkungsgrad]]*(Table1[[#This Row],[Change in Power]]+E35)-E35*F35)/Table1[[#This Row],[Change in Power]]</f>
         <v>0.58582248391959835</v>
       </c>
     </row>
@@ -1691,4 +1896,628 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7124981-34F7-41C9-B6D3-B94771EA45C3}">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <f>SUMPRODUCT(Table1[Change in Power],Table1[Angepasster Wirkungsgrad])/SUM(Table1[Change in Power])</f>
+        <v>0.62486865398920222</v>
+      </c>
+      <c r="C2">
+        <f>MAX(Table1[Angepasster Wirkungsgrad])</f>
+        <v>0.65983699477611935</v>
+      </c>
+      <c r="D2">
+        <f>_xlfn.XLOOKUP(C2,Table1[Angepasster Wirkungsgrad],Table1[Power '[%']])</f>
+        <v>0.13077384523095381</v>
+      </c>
+      <c r="E2">
+        <f>1-D2</f>
+        <v>0.86922615476904619</v>
+      </c>
+      <c r="F2">
+        <f>ROUNDUP(D2,2)</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G2">
+        <f>1-F2</f>
+        <v>0.86</v>
+      </c>
+      <c r="H2">
+        <f>E2/(A6-1)</f>
+        <v>9.6580683863227351E-2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <f>D2</f>
+        <v>0.13077384523095381</v>
+      </c>
+      <c r="K3">
+        <f>L3</f>
+        <v>0.65983699477611935</v>
+      </c>
+      <c r="L3">
+        <f>C2</f>
+        <v>0.65983699477611935</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <f>J3+$H$2</f>
+        <v>0.22735452909418116</v>
+      </c>
+      <c r="K4">
+        <f>L4/M4</f>
+        <v>0.6578833107588411</v>
+      </c>
+      <c r="L4">
+        <f>(SUMPRODUCT('Efficiency Electrolyzer'!E13:E15,'Efficiency Electrolyzer'!F13:F15)+'Efficiency Electrolyzer'!F16*('Efficiency Electrolyzer'!A16-Idea_Implementation!J4))</f>
+        <v>2.6299520078033463</v>
+      </c>
+      <c r="M4">
+        <f>(SUM('Efficiency Electrolyzer'!E13:E15)+('Efficiency Electrolyzer'!A16-Idea_Implementation!J4))</f>
+        <v>3.9975964807038586</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <f>J4+$H$2</f>
+        <v>0.32393521295740851</v>
+      </c>
+      <c r="K5">
+        <f>L5/M5</f>
+        <v>0.65100831550467586</v>
+      </c>
+      <c r="L5">
+        <f>SUMPRODUCT('Efficiency Electrolyzer'!E16:E18,'Efficiency Electrolyzer'!F16:F18)+'Efficiency Electrolyzer'!F19*('Efficiency Electrolyzer'!A19-Idea_Implementation!J4)+('Efficiency Electrolyzer'!F22*('Efficiency Electrolyzer'!A22-Idea_Implementation!J5))</f>
+        <v>3.5298670615486381</v>
+      </c>
+      <c r="M5">
+        <f>SUM('Efficiency Electrolyzer'!E16:E18)+('Efficiency Electrolyzer'!A19-Idea_Implementation!J4)+('Efficiency Electrolyzer'!A22-Idea_Implementation!J5)</f>
+        <v>5.4221535692861433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <f>J5+$H$2</f>
+        <v>0.42051589682063584</v>
+      </c>
+      <c r="K6">
+        <f>L6/M6</f>
+        <v>0.64085424326136353</v>
+      </c>
+      <c r="L6">
+        <f>SUMPRODUCT('Efficiency Electrolyzer'!E19:E21,'Efficiency Electrolyzer'!F19:F21)+'Efficiency Electrolyzer'!F19*('Efficiency Electrolyzer'!A19-Idea_Implementation!J5)+'Efficiency Electrolyzer'!F22*(Idea_Implementation!J6-'Efficiency Electrolyzer'!A21)</f>
+        <v>3.056870896000115</v>
+      </c>
+      <c r="M6">
+        <f>SUM('Efficiency Electrolyzer'!E19:E21)+('Efficiency Electrolyzer'!A19-Idea_Implementation!J5)+(Idea_Implementation!J6-'Efficiency Electrolyzer'!A21)</f>
+        <v>4.769994001199759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <f>J6+$H$2</f>
+        <v>0.51709658068386322</v>
+      </c>
+      <c r="K7">
+        <f>L7/M7</f>
+        <v>0.63298113441377046</v>
+      </c>
+      <c r="L7">
+        <f>SUMPRODUCT('Efficiency Electrolyzer'!E22:E24,'Efficiency Electrolyzer'!F22:F24)+'Efficiency Electrolyzer'!F25*(Idea_Implementation!J7-'Efficiency Electrolyzer'!A24)+'Efficiency Electrolyzer'!F22*('Efficiency Electrolyzer'!A22-Idea_Implementation!J6)</f>
+        <v>2.9101893045144349</v>
+      </c>
+      <c r="M7">
+        <f>SUM('Efficiency Electrolyzer'!E22:E24)+(Idea_Implementation!J7-'Efficiency Electrolyzer'!A24)+('Efficiency Electrolyzer'!A22-Idea_Implementation!J6)</f>
+        <v>4.5975924815037015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <f>J7+$H$2</f>
+        <v>0.6136772645470906</v>
+      </c>
+      <c r="K8">
+        <f>L8/M8</f>
+        <v>0.62107385131578929</v>
+      </c>
+      <c r="L8">
+        <f>SUMPRODUCT('Efficiency Electrolyzer'!E25:E27,'Efficiency Electrolyzer'!F25:F27)</f>
+        <v>3.3041128889999971</v>
+      </c>
+      <c r="M8">
+        <f>SUM('Efficiency Electrolyzer'!E25:E27)</f>
+        <v>5.3199999999999967</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <f>J8+$H$2</f>
+        <v>0.71025794841031797</v>
+      </c>
+      <c r="K9">
+        <f>L9/M9</f>
+        <v>0.6119388</v>
+      </c>
+      <c r="L9">
+        <f>SUMPRODUCT('Efficiency Electrolyzer'!E28:E29,'Efficiency Electrolyzer'!F28:F29)</f>
+        <v>2.5456654080000023</v>
+      </c>
+      <c r="M9">
+        <f>SUM('Efficiency Electrolyzer'!E28:E29)</f>
+        <v>4.1600000000000037</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J10">
+        <f>J9+$H$2</f>
+        <v>0.80683863227354535</v>
+      </c>
+      <c r="K10">
+        <f>L10/M10</f>
+        <v>0.60260639999999988</v>
+      </c>
+      <c r="L10">
+        <f>SUMPRODUCT('Efficiency Electrolyzer'!E30:E31,'Efficiency Electrolyzer'!F30:F31)</f>
+        <v>2.9407192319999966</v>
+      </c>
+      <c r="M10">
+        <f>SUM('Efficiency Electrolyzer'!E30:E31)</f>
+        <v>4.8799999999999955</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J11">
+        <f>J10+$H$2</f>
+        <v>0.90341931613677273</v>
+      </c>
+      <c r="K11">
+        <f>L11/M11</f>
+        <v>0.5946072</v>
+      </c>
+      <c r="L11">
+        <f>SUMPRODUCT('Efficiency Electrolyzer'!E32:E33,'Efficiency Electrolyzer'!F32:F33)</f>
+        <v>2.7827616959999997</v>
+      </c>
+      <c r="M11">
+        <f>SUM('Efficiency Electrolyzer'!E32:E33)</f>
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J12">
+        <f>J11+$H$2</f>
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <f>L12/M12</f>
+        <v>0.58701176275167799</v>
+      </c>
+      <c r="L12">
+        <f>SUMPRODUCT('Efficiency Electrolyzer'!E34:E36,'Efficiency Electrolyzer'!F34:F36)</f>
+        <v>3.4985901060000013</v>
+      </c>
+      <c r="M12">
+        <f>SUM('Efficiency Electrolyzer'!E34:E36)</f>
+        <v>5.9600000000000009</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B46336-320B-4C33-8699-FE07FFD4BAD0}">
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.69443393780398899</v>
+      </c>
+      <c r="E2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>5.198960207958409E-3</v>
+      </c>
+      <c r="B3">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.69970374927393175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1.2797440511897622E-2</v>
+      </c>
+      <c r="B4">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.70787868495044581</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2.0595880823835233E-2</v>
+      </c>
+      <c r="B5">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.71164215848150347</v>
+      </c>
+      <c r="E5">
+        <f>SUMPRODUCT(Table1[Change in Power],B2:B36)/SUM(Table1[Change in Power])</f>
+        <v>0.69999999999999973</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2.8194361127774445E-2</v>
+      </c>
+      <c r="B6">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.7169575798604203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>3.5992801439712063E-2</v>
+      </c>
+      <c r="B7">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.72122543644203252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>4.8790241951609678E-2</v>
+      </c>
+      <c r="B8">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.72564744068452713</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6.4187162567486508E-2</v>
+      </c>
+      <c r="B9">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.73146967299770838</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8.3383323335332937E-2</v>
+      </c>
+      <c r="B10">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.7347815024906561</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>0.10397920415916817</v>
+      </c>
+      <c r="B11">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.73770456992462785</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0.13077384523095381</v>
+      </c>
+      <c r="B12">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.73917277398149805</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>0.15396920615876825</v>
+      </c>
+      <c r="B13">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.73779760104157355</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>0.18216356728654268</v>
+      </c>
+      <c r="B14">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.73846054845334541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>0.21035792841431714</v>
+      </c>
+      <c r="B15">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.73487509436145404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>0.24495100979804041</v>
+      </c>
+      <c r="B16">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.73406283308106746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>0.27814437112577484</v>
+      </c>
+      <c r="B17">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.72794525406325983</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>0.31413717256548696</v>
+      </c>
+      <c r="B18">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.72748695814910991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>0.34233153369326136</v>
+      </c>
+      <c r="B19">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.7203373226003863</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>0.37832433513297348</v>
+      </c>
+      <c r="B20">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.72082844683887259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0.40891821635672865</v>
+      </c>
+      <c r="B21">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.71223253691063981</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0.44111177764447107</v>
+      </c>
+      <c r="B22">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.71401257197695622</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>0.47190561887622479</v>
+      </c>
+      <c r="B23">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.70536497900183681</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>0.50009998000399924</v>
+      </c>
+      <c r="B24">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.70758168570183322</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>0.53069386122775442</v>
+      </c>
+      <c r="B25">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.69890087215424312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>0.5654869026194761</v>
+      </c>
+      <c r="B26">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.69900635443802284</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>0.60647870425914818</v>
+      </c>
+      <c r="B27">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.69063166041969115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>0.64867026594681065</v>
+      </c>
+      <c r="B28">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.68864230952543704</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>0.68966206758648274</v>
+      </c>
+      <c r="B29">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.6822972138031479</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>0.73725254949010199</v>
+      </c>
+      <c r="B30">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.67855789033636216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>0.78724255148970201</v>
+      </c>
+      <c r="B31">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.67173202777947794</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>0.83583283343331327</v>
+      </c>
+      <c r="B32">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.66939588367004732</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>0.88082383523295338</v>
+      </c>
+      <c r="B33">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.66254054409193275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>0.92561487702459511</v>
+      </c>
+      <c r="B34">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.6614428676112506</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>0.96020795840831841</v>
+      </c>
+      <c r="B35">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.65413695678523431</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <f>Table1[[#This Row],[Angepasster Wirkungsgrad]]*(Test_Adjustment!$E$2/Idea_Implementation!$A$2)</f>
+        <v>0.65625909721310005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F4518F-E053-4336-B711-7AA8B14FF1BD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
improve calculation of adjusted efficiencies
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzer.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Efficiency_Electrolyzer.xlsx
@@ -1,51 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="13_ncr:1_{046BDF9C-14DC-4C73-8529-F59D1FAC7293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{733D4EFB-DBC6-4682-AB89-677C695FC063}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1E7DE9-F77E-441C-8EF4-11DE7372B8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-11505" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Efficiency Electrolyzer" sheetId="1" r:id="rId1"/>
-    <sheet name="Idea_Implementation" sheetId="3" r:id="rId2"/>
-    <sheet name="Test_Adjustment" sheetId="4" r:id="rId3"/>
-    <sheet name="Source" sheetId="2" r:id="rId4"/>
+    <sheet name="efficiency_raw" sheetId="5" r:id="rId1"/>
+    <sheet name="Efficiency Electrolyzer" sheetId="1" r:id="rId2"/>
+    <sheet name="Idea_Implementation" sheetId="3" r:id="rId3"/>
+    <sheet name="Test_Adjustment" sheetId="4" r:id="rId4"/>
+    <sheet name="Source" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Efficiency Electrolyzer'!#REF!</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">"0,0001"</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="0" hidden="1">"0,075"</definedName>
-    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Efficiency Electrolyzer'!#REF!</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">"0,000001"</definedName>
-    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Efficiency Electrolyzer'!#REF!</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">"0,0001"</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">"0,075"</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Efficiency Electrolyzer'!#REF!</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">"0,000001"</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Efficiency [kg/MWh]</t>
   </si>
@@ -116,6 +117,9 @@
   </si>
   <si>
     <t>EFF</t>
+  </si>
+  <si>
+    <t>Efficiency [%]</t>
   </si>
 </sst>
 </file>
@@ -716,9 +720,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -756,7 +760,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -862,7 +866,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1004,19 +1008,463 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2433A841-7153-44ED-9730-8ADB27239D68}">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2*33.33/1000</f>
+        <v>0.61993799999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>5.1989999999999996E-3</v>
+      </c>
+      <c r="B3">
+        <v>18.739999999999998</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C36" si="0">B3*33.33/1000</f>
+        <v>0.62460419999999983</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1.2796999999999999E-2</v>
+      </c>
+      <c r="B4">
+        <v>18.87</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.62893710000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2.0596E-2</v>
+      </c>
+      <c r="B5">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.63360329999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2.8194E-2</v>
+      </c>
+      <c r="B6">
+        <v>19.13</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.63760289999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>3.5992999999999997E-2</v>
+      </c>
+      <c r="B7">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.64193579999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>4.879E-2</v>
+      </c>
+      <c r="B8">
+        <v>19.39</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.64626869999999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6.4186999999999994E-2</v>
+      </c>
+      <c r="B9">
+        <v>19.52</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.6506016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8.3382999999999999E-2</v>
+      </c>
+      <c r="B10">
+        <v>19.64</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.65460119999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>0.103979</v>
+      </c>
+      <c r="B11">
+        <v>19.72</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.65726759999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0.130774</v>
+      </c>
+      <c r="B12">
+        <v>19.78</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.65926739999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>0.15396899999999999</v>
+      </c>
+      <c r="B13">
+        <v>19.78</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.65926739999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>0.18216399999999999</v>
+      </c>
+      <c r="B14">
+        <v>19.77</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.65893409999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>0.21035799999999999</v>
+      </c>
+      <c r="B15">
+        <v>19.73</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.65760090000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>0.244951</v>
+      </c>
+      <c r="B16">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.65560109999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>0.278144</v>
+      </c>
+      <c r="B17">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.65260139999999989</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>0.314137</v>
+      </c>
+      <c r="B18">
+        <v>19.489999999999998</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="0"/>
+        <v>0.64960169999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>0.34233200000000003</v>
+      </c>
+      <c r="B19">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.64660200000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>0.37832399999999999</v>
+      </c>
+      <c r="B20">
+        <v>19.3</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.64326899999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0.408918</v>
+      </c>
+      <c r="B21">
+        <v>19.2</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="0"/>
+        <v>0.63993599999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0.441112</v>
+      </c>
+      <c r="B22">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>0.63660300000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>0.47190599999999999</v>
+      </c>
+      <c r="B23">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>0.63360329999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>0.50009999999999999</v>
+      </c>
+      <c r="B24">
+        <v>18.920000000000002</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>0.63060360000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>0.530694</v>
+      </c>
+      <c r="B25">
+        <v>18.829999999999998</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>0.62760389999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>0.56548699999999996</v>
+      </c>
+      <c r="B26">
+        <v>18.72</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="0"/>
+        <v>0.62393759999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>0.60647899999999999</v>
+      </c>
+      <c r="B27">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="0"/>
+        <v>0.61993799999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>0.64866999999999997</v>
+      </c>
+      <c r="B28">
+        <v>18.47</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="0"/>
+        <v>0.61560509999999991</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>0.689662</v>
+      </c>
+      <c r="B29">
+        <v>18.36</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.61193879999999989</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>0.73725300000000005</v>
+      </c>
+      <c r="B30">
+        <v>18.22</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="0"/>
+        <v>0.60727259999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>0.78724300000000003</v>
+      </c>
+      <c r="B31">
+        <v>18.079999999999998</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="0"/>
+        <v>0.60260639999999988</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>0.83583300000000005</v>
+      </c>
+      <c r="B32">
+        <v>17.96</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="0"/>
+        <v>0.59860679999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>0.88082400000000005</v>
+      </c>
+      <c r="B33">
+        <v>17.84</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="0"/>
+        <v>0.59460719999999989</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>0.92561499999999997</v>
+      </c>
+      <c r="B34">
+        <v>17.73</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="0"/>
+        <v>0.59094089999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>0.96020799999999995</v>
+      </c>
+      <c r="B35">
+        <v>17.63</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="0"/>
+        <v>0.58760789999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>17.55</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5849415</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1349,7 +1797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7124981-34F7-41C9-B6D3-B94771EA45C3}">
   <dimension ref="A1:M12"/>
   <sheetViews>
@@ -1602,7 +2050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B46336-320B-4C33-8699-FE07FFD4BAD0}">
   <dimension ref="A1:E36"/>
   <sheetViews>
@@ -1953,7 +2401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F4518F-E053-4336-B711-7AA8B14FF1BD}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>